<commit_message>
Fixed tables on Resources page
</commit_message>
<xml_diff>
--- a/content/single_cell_RNA-seq.xlsx
+++ b/content/single_cell_RNA-seq.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhenadmin\Documents\Scripts\my_web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Users\Zhen\Documents\zhen\scripts\zhenli.name\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14820" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14820"/>
   </bookViews>
   <sheets>
     <sheet name="Human" sheetId="1" r:id="rId1"/>
@@ -145,30 +145,6 @@
     <t>2M</t>
   </si>
   <si>
-    <t>&lt;a href="https://www.nature.com/articles/nn.3980"&gt;Johnson&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="http://www.pnas.org/content/112/23/7285"&gt;Darmanis&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="http://science.sciencemag.org/content/352/6293/1586.long"&gt;Lake&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://doi.org/10.1016/j.cell.2015.09.004"&gt;Pollen&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="http://science.sciencemag.org/content/358/6368/1318"&gt;Nowakowski&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://www.nature.com/articles/nature25980"&gt;Zhong&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://www.nature.com/articles/nbt.4038"&gt;Lake&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://www.nature.com/articles/s41422-018-0053-3"&gt;Fan&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>P25</t>
   </si>
   <si>
@@ -281,6 +257,30 @@
   </si>
   <si>
     <t>Genes/cell</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.nature.com/articles/nn.3980" target="_blank"&gt;Johnson&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://www.pnas.org/content/112/23/7285" target="_blank"&gt;Darmanis&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://science.sciencemag.org/content/352/6293/1586.long"  target="_blank"&gt;Lake&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://doi.org/10.1016/j.cell.2015.09.004"  target="_blank"&gt;Pollen&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://science.sciencemag.org/content/358/6368/1318"  target="_blank"&gt;Nowakowski&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.nature.com/articles/nature25980"  target="_blank"&gt;Zhong&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.nature.com/articles/nbt.4038"  target="_blank"&gt;Lake&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.nature.com/articles/s41422-018-0053-3"  target="_blank"&gt;Fan&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -601,16 +601,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -633,12 +633,12 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -662,9 +662,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -688,9 +688,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -714,9 +714,9 @@
         <v>6159</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -740,9 +740,9 @@
         <v>3099</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -766,9 +766,9 @@
         <v>2403</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -792,9 +792,9 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -818,9 +818,9 @@
         <v>719</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
         <v>35</v>
@@ -857,14 +857,14 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="92.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -878,21 +878,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -901,76 +901,76 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H2">
         <v>4717</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1">
         <v>1679</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H3">
         <v>7278</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E4" s="1">
         <v>3005</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H4" s="1">
         <v>4500</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -979,13 +979,13 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1">
         <v>44808</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -994,18 +994,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E6" s="1">
         <v>156049</v>
@@ -1020,50 +1020,50 @@
         <v>4497</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E7" s="1">
         <v>1916</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H7" s="1">
         <v>6361</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -1072,24 +1072,24 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E9" s="1">
         <v>396</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -1107,16 +1107,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1130,18 +1130,18 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -1150,7 +1150,7 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E2">
         <v>82291</v>

</xml_diff>

<commit_message>
Added one paper to database
</commit_message>
<xml_diff>
--- a/content/single_cell_RNA-seq.xlsx
+++ b/content/single_cell_RNA-seq.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Human" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="96">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -174,7 +174,35 @@
     <t xml:space="preserve">Source</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;a href="https://www.nature.com/articles/srep18178"&gt;Saraiva&lt;/a&gt;</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;a href="https://www.nature.com/articles/srep18178" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target=”_blank”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;Saraiva&lt;/a&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">P25</t>
@@ -186,7 +214,35 @@
     <t xml:space="preserve">4.4M</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;a href="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4985242/"&gt;Tasic&lt;/a&gt;</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;a href="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4985242/" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target=”_blank”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;Tasic&lt;/a&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">SMARTer</t>
@@ -201,7 +257,35 @@
     <t xml:space="preserve">8.7M</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;a href="http://science.sciencemag.org/content/347/6226/1138"&gt;Zeisel&lt;/a&gt;</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;a href="http://science.sciencemag.org/content/347/6226/1138" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target=”_blank”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;Zeisel&lt;/a&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">5'</t>
@@ -216,7 +300,35 @@
     <t xml:space="preserve">0.5M</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0092867415005498"&gt;Macosko&lt;/a&gt;</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0092867415005498" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target=”_blank”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;Macosko&lt;/a&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">P14</t>
@@ -225,7 +337,35 @@
     <t xml:space="preserve">Retina</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;a href="http://science.sciencemag.org/content/360/6385/176"&gt;Rosenberg&lt;/a&gt;</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;a href="http://science.sciencemag.org/content/360/6385/176" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target=”_blank”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;Rosenberg&lt;/a&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">SPLiT-seq</t>
@@ -237,7 +377,35 @@
     <t xml:space="preserve">P2 &amp; P11</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;a href="https://genomebiology.biomedcentral.com/articles/10.1186/s13059-018-1416-2"&gt;Dong&lt;/a&gt;</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;a href="https://genomebiology.biomedcentral.com/articles/10.1186/s13059-018-1416-2" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target=”_blank”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;Dong&lt;/a&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">E9.5-11.5</t>
@@ -249,7 +417,35 @@
     <t xml:space="preserve">0.43M UMI/cell</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0092867418301168"&gt;Han&lt;/a&gt;</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0092867418301168" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target=”_blank”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;Han&lt;/a&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Microwell-seq</t>
@@ -261,7 +457,35 @@
     <t xml:space="preserve">&gt;400,000</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0002929718300466"&gt;Hook&lt;/a&gt;</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0002929718300466" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target=”_blank”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;Hook&lt;/a&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Smart-Seq2</t>
@@ -273,35 +497,25 @@
     <t xml:space="preserve">Midbrain &amp; forebrain</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;a href="https://www.nature.com/articles/nature22047" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">target=”_blank”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt;Quadrato&lt;/a&gt;</t>
-    </r>
+    <t xml:space="preserve">&lt;a href="https://www.nature.com/articles/nature25999" target=”_blank”&gt;Mayer&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop-seq &amp; 10X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E13.5, E14.5, E18.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5622, 7401, 8543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MGE, CGE, LGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;a href="https://www.nature.com/articles/nature22047" target=”_blank”&gt;Quadrato&lt;/a&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">3 and 6mons</t>
@@ -311,9 +525,6 @@
   </si>
   <si>
     <t xml:space="preserve">10X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3’</t>
   </si>
   <si>
     <t xml:space="preserve">30 and 72-79 days</t>
@@ -434,7 +645,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -693,10 +904,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -734,7 +945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>50</v>
       </c>
@@ -760,7 +971,7 @@
         <v>4717</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>54</v>
       </c>
@@ -786,7 +997,7 @@
         <v>7278</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>59</v>
       </c>
@@ -812,7 +1023,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>64</v>
       </c>
@@ -838,7 +1049,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>67</v>
       </c>
@@ -864,7 +1075,7 @@
         <v>4497</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>71</v>
       </c>
@@ -890,7 +1101,7 @@
         <v>6361</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>75</v>
       </c>
@@ -916,7 +1127,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>79</v>
       </c>
@@ -942,7 +1153,44 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1626</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.nature.com/articles/srep18178"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4985242/"/>
+    <hyperlink ref="A4" r:id="rId3" display="http://science.sciencemag.org/content/347/6226/1138"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://www.sciencedirect.com/science/article/pii/S0092867415005498"/>
+    <hyperlink ref="A6" r:id="rId5" display="http://science.sciencemag.org/content/360/6385/176"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://genomebiology.biomedcentral.com/articles/10.1186/s13059-018-1416-2"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://www.sciencedirect.com/science/article/pii/S0092867418301168"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://www.sciencedirect.com/science/article/pii/S0002929718300466"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://www.nature.com/articles/nature25999"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -960,7 +1208,7 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -995,7 +1243,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>39</v>
@@ -1004,7 +1252,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>82291</v>
@@ -1018,16 +1266,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>87</v>
-      </c>
       <c r="D3" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>59235</v>
@@ -1041,16 +1289,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>3850</v>
@@ -1064,8 +1312,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.nature.com/articles/nature22047"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://www.sciencedirect.com/science/article/pii/S1934590917302862"/>
+    <hyperlink ref="A2" r:id="rId1" display="&lt;a href=&quot;https://www.nature.com/articles/nature22047&quot; target=”_blank”&gt;Quadrato&lt;/a&gt;"/>
+    <hyperlink ref="A3" r:id="rId2" display="&lt;a href=&quot;https://www.sciencedirect.com/science/article/pii/S1934590917302862&quot; target=”_blank”&gt;Xiang&lt;/a&gt;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added one post and one entry in resource
</commit_message>
<xml_diff>
--- a/content/single_cell_RNA-seq.xlsx
+++ b/content/single_cell_RNA-seq.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="100">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -174,35 +174,7 @@
     <t xml:space="preserve">Source</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;a href="https://www.nature.com/articles/srep18178" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">target=”_blank”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt;Saraiva&lt;/a&gt;</t>
-    </r>
+    <t xml:space="preserve">&lt;a href="https://www.nature.com/articles/srep18178" target=”_blank”&gt;Saraiva&lt;/a&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">P25</t>
@@ -214,35 +186,7 @@
     <t xml:space="preserve">4.4M</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;a href="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4985242/" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">target=”_blank”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt;Tasic&lt;/a&gt;</t>
-    </r>
+    <t xml:space="preserve">&lt;a href="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4985242/" target=”_blank”&gt;Tasic&lt;/a&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">SMARTer</t>
@@ -257,35 +201,7 @@
     <t xml:space="preserve">8.7M</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;a href="http://science.sciencemag.org/content/347/6226/1138" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">target=”_blank”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt;Zeisel&lt;/a&gt;</t>
-    </r>
+    <t xml:space="preserve">&lt;a href="http://science.sciencemag.org/content/347/6226/1138" target=”_blank”&gt;Zeisel&lt;/a&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">5'</t>
@@ -300,35 +216,7 @@
     <t xml:space="preserve">0.5M</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0092867415005498" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">target=”_blank”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt;Macosko&lt;/a&gt;</t>
-    </r>
+    <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0092867415005498" target=”_blank”&gt;Macosko&lt;/a&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">P14</t>
@@ -337,35 +225,7 @@
     <t xml:space="preserve">Retina</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;a href="http://science.sciencemag.org/content/360/6385/176" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">target=”_blank”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt;Rosenberg&lt;/a&gt;</t>
-    </r>
+    <t xml:space="preserve">&lt;a href="http://science.sciencemag.org/content/360/6385/176" target=”_blank”&gt;Rosenberg&lt;/a&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">SPLiT-seq</t>
@@ -377,35 +237,7 @@
     <t xml:space="preserve">P2 &amp; P11</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;a href="https://genomebiology.biomedcentral.com/articles/10.1186/s13059-018-1416-2" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">target=”_blank”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt;Dong&lt;/a&gt;</t>
-    </r>
+    <t xml:space="preserve">&lt;a href="https://genomebiology.biomedcentral.com/articles/10.1186/s13059-018-1416-2" target=”_blank”&gt;Dong&lt;/a&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">E9.5-11.5</t>
@@ -417,35 +249,7 @@
     <t xml:space="preserve">0.43M UMI/cell</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0092867418301168" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">target=”_blank”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt;Han&lt;/a&gt;</t>
-    </r>
+    <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0092867418301168" target=”_blank”&gt;Han&lt;/a&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Microwell-seq</t>
@@ -457,35 +261,7 @@
     <t xml:space="preserve">&gt;400,000</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0002929718300466" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">target=”_blank”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt;Hook&lt;/a&gt;</t>
-    </r>
+    <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0002929718300466" target=”_blank”&gt;Hook&lt;/a&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Smart-Seq2</t>
@@ -513,6 +289,18 @@
   </si>
   <si>
     <t xml:space="preserve">MGE, CGE, LGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;a href=”https://www.sciencedirect.com/science/article/pii/S1074761318304850?via%3Dihub” target=”_blank”&gt;Hammond&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E14.5, P4/5, P30, P100, P540, injury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microglia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40,000 – 60,000 reads / sample</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;a href="https://www.nature.com/articles/nature22047" target=”_blank”&gt;Quadrato&lt;/a&gt;</t>
@@ -544,7 +332,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -566,12 +354,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -904,10 +686,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1153,7 +935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>83</v>
       </c>
@@ -1179,17 +961,43 @@
         <v>1626</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>76149</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.nature.com/articles/srep18178"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4985242/"/>
-    <hyperlink ref="A4" r:id="rId3" display="http://science.sciencemag.org/content/347/6226/1138"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://www.sciencedirect.com/science/article/pii/S0092867415005498"/>
-    <hyperlink ref="A6" r:id="rId5" display="http://science.sciencemag.org/content/360/6385/176"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://genomebiology.biomedcentral.com/articles/10.1186/s13059-018-1416-2"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://www.sciencedirect.com/science/article/pii/S0092867418301168"/>
-    <hyperlink ref="A9" r:id="rId8" display="https://www.sciencedirect.com/science/article/pii/S0002929718300466"/>
-    <hyperlink ref="A10" r:id="rId9" display="https://www.nature.com/articles/nature25999"/>
+    <hyperlink ref="A2" r:id="rId1" display="&lt;a href=&quot;https://www.nature.com/articles/srep18178&quot; target=”_blank”&gt;Saraiva&lt;/a&gt;"/>
+    <hyperlink ref="A3" r:id="rId2" display="&lt;a href=&quot;https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4985242/&quot; target=”_blank”&gt;Tasic&lt;/a&gt;"/>
+    <hyperlink ref="A4" r:id="rId3" display="&lt;a href=&quot;http://science.sciencemag.org/content/347/6226/1138&quot; target=”_blank”&gt;Zeisel&lt;/a&gt;"/>
+    <hyperlink ref="A5" r:id="rId4" display="&lt;a href=&quot;https://www.sciencedirect.com/science/article/pii/S0092867415005498&quot; target=”_blank”&gt;Macosko&lt;/a&gt;"/>
+    <hyperlink ref="A6" r:id="rId5" display="&lt;a href=&quot;http://science.sciencemag.org/content/360/6385/176&quot; target=”_blank”&gt;Rosenberg&lt;/a&gt;"/>
+    <hyperlink ref="A7" r:id="rId6" display="&lt;a href=&quot;https://genomebiology.biomedcentral.com/articles/10.1186/s13059-018-1416-2&quot; target=”_blank”&gt;Dong&lt;/a&gt;"/>
+    <hyperlink ref="A8" r:id="rId7" display="&lt;a href=&quot;https://www.sciencedirect.com/science/article/pii/S0092867418301168&quot; target=”_blank”&gt;Han&lt;/a&gt;"/>
+    <hyperlink ref="A9" r:id="rId8" display="&lt;a href=&quot;https://www.sciencedirect.com/science/article/pii/S0002929718300466&quot; target=”_blank”&gt;Hook&lt;/a&gt;"/>
+    <hyperlink ref="A10" r:id="rId9" display="&lt;a href=&quot;https://www.nature.com/articles/nature25999&quot; target=”_blank”&gt;Mayer&lt;/a&gt;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1243,7 +1051,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>39</v>
@@ -1252,7 +1060,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>82291</v>
@@ -1266,16 +1074,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>85</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>59235</v>
@@ -1289,16 +1097,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>85</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>3850</v>

</xml_diff>

<commit_message>
Add one entry into mouse single cell dataset table
</commit_message>
<xml_diff>
--- a/content/single_cell_RNA-seq.xlsx
+++ b/content/single_cell_RNA-seq.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="105">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -174,6 +174,9 @@
     <t xml:space="preserve">Source</t>
   </si>
   <si>
+    <t xml:space="preserve">Seq Depth/cell</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;a href="https://www.nature.com/articles/srep18178" target=”_blank”&gt;Saraiva&lt;/a&gt;</t>
   </si>
   <si>
@@ -246,7 +249,7 @@
     <t xml:space="preserve">Multiple organs</t>
   </si>
   <si>
-    <t xml:space="preserve">0.43M UMI/cell</t>
+    <t xml:space="preserve">0.43M UMI</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;a href="https://www.sciencedirect.com/science/article/pii/S0092867418301168" target=”_blank”&gt;Han&lt;/a&gt;</t>
@@ -300,7 +303,19 @@
     <t xml:space="preserve">Microglia</t>
   </si>
   <si>
-    <t xml:space="preserve">40,000 – 60,000 reads / sample</t>
+    <t xml:space="preserve">40,000 – 60,000 reads </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;a href=”https://www.nature.com/articles/s41467-018-08079-9#Bib1” target=”_blank”&gt;Loo&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E14.5, P0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,931 at E14.5; 7614 at P0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,000 reads</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;a href="https://www.nature.com/articles/nature22047" target=”_blank”&gt;Quadrato&lt;/a&gt;</t>
@@ -332,7 +347,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -354,6 +369,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -398,12 +419,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -686,10 +711,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -721,7 +746,7 @@
         <v>49</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>7</v>
@@ -729,7 +754,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>15</v>
@@ -738,16 +763,16 @@
         <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>30</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>4717</v>
@@ -755,25 +780,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1679</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>7278</v>
@@ -781,25 +806,25 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>3005</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>4500</v>
@@ -807,7 +832,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>39</v>
@@ -816,13 +841,13 @@
         <v>40</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>44808</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>12</v>
@@ -833,16 +858,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>156049</v>
@@ -859,25 +884,25 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>1916</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>6361</v>
@@ -885,22 +910,22 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>12</v>
@@ -911,22 +936,22 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>396</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>12</v>
@@ -937,22 +962,22 @@
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>12</v>
@@ -963,28 +988,54 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>76149</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1600</v>
       </c>
     </row>
   </sheetData>
@@ -1051,7 +1102,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>39</v>
@@ -1060,7 +1111,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>82291</v>
@@ -1074,16 +1125,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>59235</v>
@@ -1097,16 +1148,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>3850</v>

</xml_diff>

<commit_message>
Added a couple of new publications
</commit_message>
<xml_diff>
--- a/content/single_cell_RNA-seq.xlsx
+++ b/content/single_cell_RNA-seq.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Human" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="107">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t xml:space="preserve">2M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;a href="https://www.nature.com/articles/s41422-018-0053-3"  target="_blank"&gt;Onorati&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-20pcw</t>
   </si>
   <si>
     <t xml:space="preserve">Source</t>
@@ -347,7 +353,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -369,12 +375,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -428,7 +428,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -449,15 +449,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="A5 A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="86.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -693,6 +693,20 @@
       </c>
       <c r="H9" s="1" t="n">
         <v>4318</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -713,8 +727,8 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="A5 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -743,10 +757,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>7</v>
@@ -754,7 +768,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>15</v>
@@ -763,16 +777,16 @@
         <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>30</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>4717</v>
@@ -780,25 +794,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1679</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>7278</v>
@@ -806,25 +820,25 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>3005</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>4500</v>
@@ -832,7 +846,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>39</v>
@@ -841,13 +855,13 @@
         <v>40</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>44808</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>12</v>
@@ -858,16 +872,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>156049</v>
@@ -884,25 +898,25 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>1916</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>6361</v>
@@ -910,22 +924,22 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>12</v>
@@ -936,22 +950,22 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>396</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>12</v>
@@ -962,22 +976,22 @@
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>12</v>
@@ -988,25 +1002,25 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>76149</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>12</v>
@@ -1014,25 +1028,25 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>32</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>1600</v>
@@ -1065,10 +1079,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1102,7 +1116,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>39</v>
@@ -1111,7 +1125,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>82291</v>
@@ -1125,16 +1139,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>59235</v>
@@ -1148,16 +1162,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>3850</v>
@@ -1167,6 +1181,11 @@
       </c>
       <c r="G4" s="0" t="n">
         <v>1870</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>